<commit_message>
something that actually calculates word-internal consonant similarity continue work on the laptop with the updates I made on desktop
</commit_message>
<xml_diff>
--- a/maltese_c_feature.xlsx
+++ b/maltese_c_feature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley\PycharmProjects\segment_similarity_calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\segment_similarity_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{983A6A5C-CF2E-4D66-BCA4-FA496035CA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B522F2D-1B78-4B38-A046-A1AE5424F7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6C6B933-40EE-4CCA-8742-1A843AC07A26}"/>
+    <workbookView xWindow="-25755" yWindow="2040" windowWidth="22020" windowHeight="11310" xr2:uid="{B6C6B933-40EE-4CCA-8742-1A843AC07A26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -48,7 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Stanley:</t>
         </r>
@@ -57,7 +56,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 trill</t>
@@ -72,7 +71,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Stanley:</t>
         </r>
@@ -81,7 +80,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 n,l,r lacking place features supported by puech</t>
@@ -254,7 +253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,14 +273,22 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -301,10 +308,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -312,18 +320,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -638,7 +648,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17189527-B303-4308-AEE1-1395AC61E295}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="A7:XFD7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -714,7 +726,7 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -785,7 +797,7 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
@@ -854,7 +866,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -925,7 +937,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -996,7 +1008,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1067,7 +1079,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1136,7 +1148,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1205,7 +1217,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1274,7 +1286,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1343,7 +1355,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1414,7 +1426,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1452,7 +1464,7 @@
       <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="9" t="s">
         <v>41</v>
       </c>
       <c r="G17" s="1"/>
@@ -1462,8 +1474,11 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A2:A3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C17" r:id="rId1" xr:uid="{F334DA0E-C701-49EA-BA33-EED670DDD00F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>